<commit_message>
export +import+danh sách sinh viên đăng ký
</commit_message>
<xml_diff>
--- a/LanguageCenter/Code/TemplateExport/template_export_hoc_sinh.xlsx
+++ b/LanguageCenter/Code/TemplateExport/template_export_hoc_sinh.xlsx
@@ -30,9 +30,6 @@
     <t>Họ</t>
   </si>
   <si>
-    <t xml:space="preserve">Tên </t>
-  </si>
-  <si>
     <t>Ngày sinh</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>Danh sách học sinh</t>
+  </si>
+  <si>
+    <t>Tên</t>
   </si>
 </sst>
 </file>
@@ -121,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -132,6 +132,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,7 +418,7 @@
   <dimension ref="A1:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -423,7 +426,7 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="23" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" style="8" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="26" style="1" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" style="1" customWidth="1"/>
@@ -432,7 +435,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -443,32 +446,32 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -477,7 +480,7 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -486,7 +489,7 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -495,7 +498,7 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -504,7 +507,7 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -513,7 +516,7 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -522,7 +525,7 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -531,7 +534,7 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -540,7 +543,7 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -549,7 +552,7 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="7"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -558,7 +561,7 @@
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -567,7 +570,7 @@
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="7"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -576,7 +579,7 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -585,7 +588,7 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="D16" s="7"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -594,7 +597,7 @@
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="D17" s="7"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -603,7 +606,7 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="D18" s="7"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -612,7 +615,7 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="D19" s="7"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -621,7 +624,7 @@
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="D20" s="7"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -630,7 +633,7 @@
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -639,7 +642,7 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="D22" s="7"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -648,7 +651,7 @@
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -657,7 +660,7 @@
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="D24" s="7"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -666,7 +669,7 @@
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="D25" s="7"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -675,7 +678,7 @@
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="D26" s="7"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -684,7 +687,7 @@
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="D27" s="7"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -693,7 +696,7 @@
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="D28" s="7"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -702,7 +705,7 @@
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="D29" s="7"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -711,7 +714,7 @@
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="D30" s="7"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -720,7 +723,7 @@
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="D31" s="7"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -729,7 +732,7 @@
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="D32" s="7"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -738,7 +741,7 @@
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="D33" s="7"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -747,7 +750,7 @@
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="D34" s="7"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
@@ -756,7 +759,7 @@
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+      <c r="D35" s="7"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -765,7 +768,7 @@
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
+      <c r="D36" s="7"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -774,7 +777,7 @@
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
+      <c r="D37" s="7"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -783,7 +786,7 @@
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="D38" s="7"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -792,7 +795,7 @@
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+      <c r="D39" s="7"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -801,7 +804,7 @@
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+      <c r="D40" s="7"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -810,7 +813,7 @@
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="D41" s="7"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
@@ -819,7 +822,7 @@
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="D42" s="7"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -828,7 +831,7 @@
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="D43" s="7"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -837,7 +840,7 @@
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="D44" s="7"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -846,7 +849,7 @@
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="D45" s="7"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -855,7 +858,7 @@
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="D46" s="7"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -864,7 +867,7 @@
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="D47" s="7"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -873,7 +876,7 @@
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
+      <c r="D48" s="7"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -882,7 +885,7 @@
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+      <c r="D49" s="7"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -891,7 +894,7 @@
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="D50" s="7"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -900,7 +903,7 @@
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="D51" s="7"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -909,7 +912,7 @@
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+      <c r="D52" s="7"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
@@ -918,7 +921,7 @@
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
+      <c r="D53" s="7"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -927,7 +930,7 @@
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
+      <c r="D54" s="7"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -936,7 +939,7 @@
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
+      <c r="D55" s="7"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -945,7 +948,7 @@
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+      <c r="D56" s="7"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -954,7 +957,7 @@
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
+      <c r="D57" s="7"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
@@ -963,7 +966,7 @@
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
+      <c r="D58" s="7"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
@@ -972,7 +975,7 @@
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
+      <c r="D59" s="7"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -981,7 +984,7 @@
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
+      <c r="D60" s="7"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -990,7 +993,7 @@
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
+      <c r="D61" s="7"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
@@ -999,7 +1002,7 @@
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="D62" s="7"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
@@ -1008,7 +1011,7 @@
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
+      <c r="D63" s="7"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -1017,7 +1020,7 @@
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
+      <c r="D64" s="7"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
@@ -1026,7 +1029,7 @@
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="D65" s="7"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
@@ -1035,7 +1038,7 @@
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
+      <c r="D66" s="7"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -1044,7 +1047,7 @@
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
+      <c r="D67" s="7"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -1053,7 +1056,7 @@
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
+      <c r="D68" s="7"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -1062,7 +1065,7 @@
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
+      <c r="D69" s="7"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -1071,7 +1074,7 @@
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
+      <c r="D70" s="7"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -1080,7 +1083,7 @@
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+      <c r="D71" s="7"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
@@ -1089,7 +1092,7 @@
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+      <c r="D72" s="7"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
@@ -1098,7 +1101,7 @@
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
+      <c r="D73" s="7"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
@@ -1107,7 +1110,7 @@
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
+      <c r="D74" s="7"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
@@ -1116,7 +1119,7 @@
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
+      <c r="D75" s="7"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
@@ -1125,7 +1128,7 @@
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+      <c r="D76" s="7"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -1134,7 +1137,7 @@
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
+      <c r="D77" s="7"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
@@ -1143,7 +1146,7 @@
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
+      <c r="D78" s="7"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
@@ -1152,7 +1155,7 @@
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
+      <c r="D79" s="7"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
@@ -1161,7 +1164,7 @@
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
+      <c r="D80" s="7"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
@@ -1170,7 +1173,7 @@
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
+      <c r="D81" s="7"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
@@ -1179,7 +1182,7 @@
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
+      <c r="D82" s="7"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
@@ -1188,7 +1191,7 @@
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
+      <c r="D83" s="7"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
@@ -1197,7 +1200,7 @@
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
+      <c r="D84" s="7"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
@@ -1206,7 +1209,7 @@
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
+      <c r="D85" s="7"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
@@ -1215,7 +1218,7 @@
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
+      <c r="D86" s="7"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
@@ -1224,7 +1227,7 @@
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
+      <c r="D87" s="7"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
@@ -1233,7 +1236,7 @@
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
+      <c r="D88" s="7"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
@@ -1242,7 +1245,7 @@
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
+      <c r="D89" s="7"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
@@ -1251,7 +1254,7 @@
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
+      <c r="D90" s="7"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
@@ -1260,7 +1263,7 @@
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
+      <c r="D91" s="7"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
@@ -1269,7 +1272,7 @@
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
+      <c r="D92" s="7"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
@@ -1278,7 +1281,7 @@
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
+      <c r="D93" s="7"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
@@ -1287,7 +1290,7 @@
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
+      <c r="D94" s="7"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
@@ -1296,7 +1299,7 @@
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
+      <c r="D95" s="7"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
@@ -1305,7 +1308,7 @@
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
+      <c r="D96" s="7"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
@@ -1314,7 +1317,7 @@
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
+      <c r="D97" s="7"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
@@ -1323,7 +1326,7 @@
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
+      <c r="D98" s="7"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
@@ -1332,7 +1335,7 @@
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
+      <c r="D99" s="7"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
@@ -1341,7 +1344,7 @@
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
+      <c r="D100" s="7"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
@@ -1350,7 +1353,7 @@
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
+      <c r="D101" s="7"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
@@ -1359,7 +1362,7 @@
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
+      <c r="D102" s="7"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
       <c r="G102" s="3"/>
@@ -1368,7 +1371,7 @@
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
+      <c r="D103" s="7"/>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
@@ -1377,7 +1380,7 @@
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
+      <c r="D104" s="7"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
       <c r="G104" s="3"/>
@@ -1386,7 +1389,7 @@
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
+      <c r="D105" s="7"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
@@ -1395,7 +1398,7 @@
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
+      <c r="D106" s="7"/>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
@@ -1404,7 +1407,7 @@
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
+      <c r="D107" s="7"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
@@ -1413,7 +1416,7 @@
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
+      <c r="D108" s="7"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
       <c r="G108" s="3"/>
@@ -1422,7 +1425,7 @@
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
+      <c r="D109" s="7"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
@@ -1431,7 +1434,7 @@
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
+      <c r="D110" s="7"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
@@ -1440,7 +1443,7 @@
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
+      <c r="D111" s="7"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
@@ -1449,7 +1452,7 @@
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
+      <c r="D112" s="7"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
@@ -1458,7 +1461,7 @@
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
+      <c r="D113" s="7"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
@@ -1467,7 +1470,7 @@
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
+      <c r="D114" s="7"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
@@ -1476,7 +1479,7 @@
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
+      <c r="D115" s="7"/>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
       <c r="G115" s="3"/>
@@ -1485,7 +1488,7 @@
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
+      <c r="D116" s="7"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
       <c r="G116" s="3"/>
@@ -1494,7 +1497,7 @@
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
+      <c r="D117" s="7"/>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
@@ -1503,7 +1506,7 @@
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
+      <c r="D118" s="7"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
@@ -1512,7 +1515,7 @@
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
+      <c r="D119" s="7"/>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
@@ -1521,7 +1524,7 @@
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
+      <c r="D120" s="7"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
@@ -1530,7 +1533,7 @@
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
+      <c r="D121" s="7"/>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
@@ -1539,7 +1542,7 @@
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
+      <c r="D122" s="7"/>
       <c r="E122" s="3"/>
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
@@ -1548,7 +1551,7 @@
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
+      <c r="D123" s="7"/>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
       <c r="G123" s="3"/>
@@ -1557,7 +1560,7 @@
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
+      <c r="D124" s="7"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
       <c r="G124" s="3"/>
@@ -1566,7 +1569,7 @@
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
-      <c r="D125" s="3"/>
+      <c r="D125" s="7"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
@@ -1575,7 +1578,7 @@
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
-      <c r="D126" s="3"/>
+      <c r="D126" s="7"/>
       <c r="E126" s="3"/>
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
@@ -1584,7 +1587,7 @@
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
-      <c r="D127" s="3"/>
+      <c r="D127" s="7"/>
       <c r="E127" s="3"/>
       <c r="F127" s="3"/>
       <c r="G127" s="3"/>
@@ -1593,7 +1596,7 @@
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
-      <c r="D128" s="3"/>
+      <c r="D128" s="7"/>
       <c r="E128" s="3"/>
       <c r="F128" s="3"/>
       <c r="G128" s="3"/>
@@ -1602,7 +1605,7 @@
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
-      <c r="D129" s="3"/>
+      <c r="D129" s="7"/>
       <c r="E129" s="3"/>
       <c r="F129" s="3"/>
       <c r="G129" s="3"/>
@@ -1611,7 +1614,7 @@
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
-      <c r="D130" s="3"/>
+      <c r="D130" s="7"/>
       <c r="E130" s="3"/>
       <c r="F130" s="3"/>
       <c r="G130" s="3"/>
@@ -1620,7 +1623,7 @@
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
-      <c r="D131" s="3"/>
+      <c r="D131" s="7"/>
       <c r="E131" s="3"/>
       <c r="F131" s="3"/>
       <c r="G131" s="3"/>
@@ -1629,7 +1632,7 @@
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
-      <c r="D132" s="3"/>
+      <c r="D132" s="7"/>
       <c r="E132" s="3"/>
       <c r="F132" s="3"/>
       <c r="G132" s="3"/>
@@ -1638,7 +1641,7 @@
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
-      <c r="D133" s="3"/>
+      <c r="D133" s="7"/>
       <c r="E133" s="3"/>
       <c r="F133" s="3"/>
       <c r="G133" s="3"/>
@@ -1647,7 +1650,7 @@
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
-      <c r="D134" s="3"/>
+      <c r="D134" s="7"/>
       <c r="E134" s="3"/>
       <c r="F134" s="3"/>
       <c r="G134" s="3"/>
@@ -1656,7 +1659,7 @@
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
-      <c r="D135" s="3"/>
+      <c r="D135" s="7"/>
       <c r="E135" s="3"/>
       <c r="F135" s="3"/>
       <c r="G135" s="3"/>
@@ -1665,7 +1668,7 @@
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
-      <c r="D136" s="3"/>
+      <c r="D136" s="7"/>
       <c r="E136" s="3"/>
       <c r="F136" s="3"/>
       <c r="G136" s="3"/>
@@ -1674,7 +1677,7 @@
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
-      <c r="D137" s="3"/>
+      <c r="D137" s="7"/>
       <c r="E137" s="3"/>
       <c r="F137" s="3"/>
       <c r="G137" s="3"/>
@@ -1683,7 +1686,7 @@
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
-      <c r="D138" s="3"/>
+      <c r="D138" s="7"/>
       <c r="E138" s="3"/>
       <c r="F138" s="3"/>
       <c r="G138" s="3"/>
@@ -1692,7 +1695,7 @@
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
-      <c r="D139" s="3"/>
+      <c r="D139" s="7"/>
       <c r="E139" s="3"/>
       <c r="F139" s="3"/>
       <c r="G139" s="3"/>
@@ -1701,7 +1704,7 @@
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
-      <c r="D140" s="3"/>
+      <c r="D140" s="7"/>
       <c r="E140" s="3"/>
       <c r="F140" s="3"/>
       <c r="G140" s="3"/>
@@ -1710,7 +1713,7 @@
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
-      <c r="D141" s="3"/>
+      <c r="D141" s="7"/>
       <c r="E141" s="3"/>
       <c r="F141" s="3"/>
       <c r="G141" s="3"/>
@@ -1719,7 +1722,7 @@
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
-      <c r="D142" s="3"/>
+      <c r="D142" s="7"/>
       <c r="E142" s="3"/>
       <c r="F142" s="3"/>
       <c r="G142" s="3"/>
@@ -1728,7 +1731,7 @@
       <c r="A143" s="3"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
-      <c r="D143" s="3"/>
+      <c r="D143" s="7"/>
       <c r="E143" s="3"/>
       <c r="F143" s="3"/>
       <c r="G143" s="3"/>
@@ -1737,7 +1740,7 @@
       <c r="A144" s="3"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
-      <c r="D144" s="3"/>
+      <c r="D144" s="7"/>
       <c r="E144" s="3"/>
       <c r="F144" s="3"/>
       <c r="G144" s="3"/>
@@ -1746,7 +1749,7 @@
       <c r="A145" s="3"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
-      <c r="D145" s="3"/>
+      <c r="D145" s="7"/>
       <c r="E145" s="3"/>
       <c r="F145" s="3"/>
       <c r="G145" s="3"/>
@@ -1755,7 +1758,7 @@
       <c r="A146" s="3"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
-      <c r="D146" s="3"/>
+      <c r="D146" s="7"/>
       <c r="E146" s="3"/>
       <c r="F146" s="3"/>
       <c r="G146" s="3"/>
@@ -1764,7 +1767,7 @@
       <c r="A147" s="3"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
-      <c r="D147" s="3"/>
+      <c r="D147" s="7"/>
       <c r="E147" s="3"/>
       <c r="F147" s="3"/>
       <c r="G147" s="3"/>
@@ -1773,7 +1776,7 @@
       <c r="A148" s="3"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
-      <c r="D148" s="3"/>
+      <c r="D148" s="7"/>
       <c r="E148" s="3"/>
       <c r="F148" s="3"/>
       <c r="G148" s="3"/>
@@ -1782,7 +1785,7 @@
       <c r="A149" s="3"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
-      <c r="D149" s="3"/>
+      <c r="D149" s="7"/>
       <c r="E149" s="3"/>
       <c r="F149" s="3"/>
       <c r="G149" s="3"/>
@@ -1791,7 +1794,7 @@
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
-      <c r="D150" s="3"/>
+      <c r="D150" s="7"/>
       <c r="E150" s="3"/>
       <c r="F150" s="3"/>
       <c r="G150" s="3"/>
@@ -1800,7 +1803,7 @@
       <c r="A151" s="3"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
-      <c r="D151" s="3"/>
+      <c r="D151" s="7"/>
       <c r="E151" s="3"/>
       <c r="F151" s="3"/>
       <c r="G151" s="3"/>
@@ -1809,7 +1812,7 @@
       <c r="A152" s="3"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
-      <c r="D152" s="3"/>
+      <c r="D152" s="7"/>
       <c r="E152" s="3"/>
       <c r="F152" s="3"/>
       <c r="G152" s="3"/>
@@ -1818,7 +1821,7 @@
       <c r="A153" s="3"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
-      <c r="D153" s="3"/>
+      <c r="D153" s="7"/>
       <c r="E153" s="3"/>
       <c r="F153" s="3"/>
       <c r="G153" s="3"/>
@@ -1827,7 +1830,7 @@
       <c r="A154" s="3"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
-      <c r="D154" s="3"/>
+      <c r="D154" s="7"/>
       <c r="E154" s="3"/>
       <c r="F154" s="3"/>
       <c r="G154" s="3"/>
@@ -1836,7 +1839,7 @@
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
-      <c r="D155" s="3"/>
+      <c r="D155" s="7"/>
       <c r="E155" s="3"/>
       <c r="F155" s="3"/>
       <c r="G155" s="3"/>
@@ -1845,7 +1848,7 @@
       <c r="A156" s="3"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
-      <c r="D156" s="3"/>
+      <c r="D156" s="7"/>
       <c r="E156" s="3"/>
       <c r="F156" s="3"/>
       <c r="G156" s="3"/>
@@ -1854,7 +1857,7 @@
       <c r="A157" s="3"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
-      <c r="D157" s="3"/>
+      <c r="D157" s="7"/>
       <c r="E157" s="3"/>
       <c r="F157" s="3"/>
       <c r="G157" s="3"/>
@@ -1863,7 +1866,7 @@
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
-      <c r="D158" s="3"/>
+      <c r="D158" s="7"/>
       <c r="E158" s="3"/>
       <c r="F158" s="3"/>
       <c r="G158" s="3"/>
@@ -1872,7 +1875,7 @@
       <c r="A159" s="3"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
-      <c r="D159" s="3"/>
+      <c r="D159" s="7"/>
       <c r="E159" s="3"/>
       <c r="F159" s="3"/>
       <c r="G159" s="3"/>
@@ -1881,7 +1884,7 @@
       <c r="A160" s="3"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
-      <c r="D160" s="3"/>
+      <c r="D160" s="7"/>
       <c r="E160" s="3"/>
       <c r="F160" s="3"/>
       <c r="G160" s="3"/>
@@ -1890,7 +1893,7 @@
       <c r="A161" s="3"/>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
-      <c r="D161" s="3"/>
+      <c r="D161" s="7"/>
       <c r="E161" s="3"/>
       <c r="F161" s="3"/>
       <c r="G161" s="3"/>
@@ -1899,7 +1902,7 @@
       <c r="A162" s="3"/>
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
-      <c r="D162" s="3"/>
+      <c r="D162" s="7"/>
       <c r="E162" s="3"/>
       <c r="F162" s="3"/>
       <c r="G162" s="3"/>
@@ -1908,7 +1911,7 @@
       <c r="A163" s="3"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
-      <c r="D163" s="3"/>
+      <c r="D163" s="7"/>
       <c r="E163" s="3"/>
       <c r="F163" s="3"/>
       <c r="G163" s="3"/>
@@ -1917,7 +1920,7 @@
       <c r="A164" s="3"/>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
-      <c r="D164" s="3"/>
+      <c r="D164" s="7"/>
       <c r="E164" s="3"/>
       <c r="F164" s="3"/>
       <c r="G164" s="3"/>
@@ -1926,7 +1929,7 @@
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
-      <c r="D165" s="3"/>
+      <c r="D165" s="7"/>
       <c r="E165" s="3"/>
       <c r="F165" s="3"/>
       <c r="G165" s="3"/>
@@ -1935,7 +1938,7 @@
       <c r="A166" s="3"/>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
-      <c r="D166" s="3"/>
+      <c r="D166" s="7"/>
       <c r="E166" s="3"/>
       <c r="F166" s="3"/>
       <c r="G166" s="3"/>
@@ -1944,7 +1947,7 @@
       <c r="A167" s="3"/>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
-      <c r="D167" s="3"/>
+      <c r="D167" s="7"/>
       <c r="E167" s="3"/>
       <c r="F167" s="3"/>
       <c r="G167" s="3"/>
@@ -1953,7 +1956,7 @@
       <c r="A168" s="3"/>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
-      <c r="D168" s="3"/>
+      <c r="D168" s="7"/>
       <c r="E168" s="3"/>
       <c r="F168" s="3"/>
       <c r="G168" s="3"/>
@@ -1962,7 +1965,7 @@
       <c r="A169" s="3"/>
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
-      <c r="D169" s="3"/>
+      <c r="D169" s="7"/>
       <c r="E169" s="3"/>
       <c r="F169" s="3"/>
       <c r="G169" s="3"/>
@@ -1971,7 +1974,7 @@
       <c r="A170" s="3"/>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
-      <c r="D170" s="3"/>
+      <c r="D170" s="7"/>
       <c r="E170" s="3"/>
       <c r="F170" s="3"/>
       <c r="G170" s="3"/>
@@ -1980,7 +1983,7 @@
       <c r="A171" s="3"/>
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
-      <c r="D171" s="3"/>
+      <c r="D171" s="7"/>
       <c r="E171" s="3"/>
       <c r="F171" s="3"/>
       <c r="G171" s="3"/>
@@ -1989,7 +1992,7 @@
       <c r="A172" s="3"/>
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
-      <c r="D172" s="3"/>
+      <c r="D172" s="7"/>
       <c r="E172" s="3"/>
       <c r="F172" s="3"/>
       <c r="G172" s="3"/>
@@ -1998,7 +2001,7 @@
       <c r="A173" s="3"/>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
-      <c r="D173" s="3"/>
+      <c r="D173" s="7"/>
       <c r="E173" s="3"/>
       <c r="F173" s="3"/>
       <c r="G173" s="3"/>
@@ -2007,7 +2010,7 @@
       <c r="A174" s="3"/>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
-      <c r="D174" s="3"/>
+      <c r="D174" s="7"/>
       <c r="E174" s="3"/>
       <c r="F174" s="3"/>
       <c r="G174" s="3"/>
@@ -2016,7 +2019,7 @@
       <c r="A175" s="3"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
-      <c r="D175" s="3"/>
+      <c r="D175" s="7"/>
       <c r="E175" s="3"/>
       <c r="F175" s="3"/>
       <c r="G175" s="3"/>
@@ -2025,7 +2028,7 @@
       <c r="A176" s="3"/>
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>
-      <c r="D176" s="3"/>
+      <c r="D176" s="7"/>
       <c r="E176" s="3"/>
       <c r="F176" s="3"/>
       <c r="G176" s="3"/>
@@ -2034,7 +2037,7 @@
       <c r="A177" s="3"/>
       <c r="B177" s="3"/>
       <c r="C177" s="3"/>
-      <c r="D177" s="3"/>
+      <c r="D177" s="7"/>
       <c r="E177" s="3"/>
       <c r="F177" s="3"/>
       <c r="G177" s="3"/>
@@ -2043,7 +2046,7 @@
       <c r="A178" s="3"/>
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
-      <c r="D178" s="3"/>
+      <c r="D178" s="7"/>
       <c r="E178" s="3"/>
       <c r="F178" s="3"/>
       <c r="G178" s="3"/>
@@ -2052,7 +2055,7 @@
       <c r="A179" s="3"/>
       <c r="B179" s="3"/>
       <c r="C179" s="3"/>
-      <c r="D179" s="3"/>
+      <c r="D179" s="7"/>
       <c r="E179" s="3"/>
       <c r="F179" s="3"/>
       <c r="G179" s="3"/>
@@ -2061,7 +2064,7 @@
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
-      <c r="D180" s="3"/>
+      <c r="D180" s="7"/>
       <c r="E180" s="3"/>
       <c r="F180" s="3"/>
       <c r="G180" s="3"/>
@@ -2070,7 +2073,7 @@
       <c r="A181" s="3"/>
       <c r="B181" s="3"/>
       <c r="C181" s="3"/>
-      <c r="D181" s="3"/>
+      <c r="D181" s="7"/>
       <c r="E181" s="3"/>
       <c r="F181" s="3"/>
       <c r="G181" s="3"/>
@@ -2079,7 +2082,7 @@
       <c r="A182" s="3"/>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
-      <c r="D182" s="3"/>
+      <c r="D182" s="7"/>
       <c r="E182" s="3"/>
       <c r="F182" s="3"/>
       <c r="G182" s="3"/>
@@ -2088,7 +2091,7 @@
       <c r="A183" s="3"/>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
-      <c r="D183" s="3"/>
+      <c r="D183" s="7"/>
       <c r="E183" s="3"/>
       <c r="F183" s="3"/>
       <c r="G183" s="3"/>
@@ -2097,7 +2100,7 @@
       <c r="A184" s="3"/>
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
-      <c r="D184" s="3"/>
+      <c r="D184" s="7"/>
       <c r="E184" s="3"/>
       <c r="F184" s="3"/>
       <c r="G184" s="3"/>
@@ -2106,7 +2109,7 @@
       <c r="A185" s="3"/>
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
-      <c r="D185" s="3"/>
+      <c r="D185" s="7"/>
       <c r="E185" s="3"/>
       <c r="F185" s="3"/>
       <c r="G185" s="3"/>
@@ -2115,7 +2118,7 @@
       <c r="A186" s="3"/>
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
-      <c r="D186" s="3"/>
+      <c r="D186" s="7"/>
       <c r="E186" s="3"/>
       <c r="F186" s="3"/>
       <c r="G186" s="3"/>
@@ -2124,7 +2127,7 @@
       <c r="A187" s="3"/>
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
-      <c r="D187" s="3"/>
+      <c r="D187" s="7"/>
       <c r="E187" s="3"/>
       <c r="F187" s="3"/>
       <c r="G187" s="3"/>
@@ -2133,7 +2136,7 @@
       <c r="A188" s="3"/>
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
-      <c r="D188" s="3"/>
+      <c r="D188" s="7"/>
       <c r="E188" s="3"/>
       <c r="F188" s="3"/>
       <c r="G188" s="3"/>
@@ -2142,7 +2145,7 @@
       <c r="A189" s="3"/>
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
-      <c r="D189" s="3"/>
+      <c r="D189" s="7"/>
       <c r="E189" s="3"/>
       <c r="F189" s="3"/>
       <c r="G189" s="3"/>
@@ -2151,7 +2154,7 @@
       <c r="A190" s="3"/>
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
-      <c r="D190" s="3"/>
+      <c r="D190" s="7"/>
       <c r="E190" s="3"/>
       <c r="F190" s="3"/>
       <c r="G190" s="3"/>
@@ -2160,7 +2163,7 @@
       <c r="A191" s="3"/>
       <c r="B191" s="3"/>
       <c r="C191" s="3"/>
-      <c r="D191" s="3"/>
+      <c r="D191" s="7"/>
       <c r="E191" s="3"/>
       <c r="F191" s="3"/>
       <c r="G191" s="3"/>
@@ -2169,7 +2172,7 @@
       <c r="A192" s="3"/>
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
-      <c r="D192" s="3"/>
+      <c r="D192" s="7"/>
       <c r="E192" s="3"/>
       <c r="F192" s="3"/>
       <c r="G192" s="3"/>
@@ -2178,7 +2181,7 @@
       <c r="A193" s="3"/>
       <c r="B193" s="3"/>
       <c r="C193" s="3"/>
-      <c r="D193" s="3"/>
+      <c r="D193" s="7"/>
       <c r="E193" s="3"/>
       <c r="F193" s="3"/>
       <c r="G193" s="3"/>
@@ -2187,7 +2190,7 @@
       <c r="A194" s="3"/>
       <c r="B194" s="3"/>
       <c r="C194" s="3"/>
-      <c r="D194" s="3"/>
+      <c r="D194" s="7"/>
       <c r="E194" s="3"/>
       <c r="F194" s="3"/>
       <c r="G194" s="3"/>
@@ -2196,7 +2199,7 @@
       <c r="A195" s="3"/>
       <c r="B195" s="3"/>
       <c r="C195" s="3"/>
-      <c r="D195" s="3"/>
+      <c r="D195" s="7"/>
       <c r="E195" s="3"/>
       <c r="F195" s="3"/>
       <c r="G195" s="3"/>
@@ -2205,7 +2208,7 @@
       <c r="A196" s="3"/>
       <c r="B196" s="3"/>
       <c r="C196" s="3"/>
-      <c r="D196" s="3"/>
+      <c r="D196" s="7"/>
       <c r="E196" s="3"/>
       <c r="F196" s="3"/>
       <c r="G196" s="3"/>
@@ -2214,7 +2217,7 @@
       <c r="A197" s="3"/>
       <c r="B197" s="3"/>
       <c r="C197" s="3"/>
-      <c r="D197" s="3"/>
+      <c r="D197" s="7"/>
       <c r="E197" s="3"/>
       <c r="F197" s="3"/>
       <c r="G197" s="3"/>
@@ -2223,7 +2226,7 @@
       <c r="A198" s="3"/>
       <c r="B198" s="3"/>
       <c r="C198" s="3"/>
-      <c r="D198" s="3"/>
+      <c r="D198" s="7"/>
       <c r="E198" s="3"/>
       <c r="F198" s="3"/>
       <c r="G198" s="3"/>
@@ -2232,7 +2235,7 @@
       <c r="A199" s="3"/>
       <c r="B199" s="3"/>
       <c r="C199" s="3"/>
-      <c r="D199" s="3"/>
+      <c r="D199" s="7"/>
       <c r="E199" s="3"/>
       <c r="F199" s="3"/>
       <c r="G199" s="3"/>
@@ -2241,7 +2244,7 @@
       <c r="A200" s="3"/>
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
-      <c r="D200" s="3"/>
+      <c r="D200" s="7"/>
       <c r="E200" s="3"/>
       <c r="F200" s="3"/>
       <c r="G200" s="3"/>

</xml_diff>